<commit_message>
Rename an error message to "Field 'XXX' is not found" format
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/NonExistingVariableInTBasic.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/NonExistingVariableInTBasic.xlsx
@@ -1,18 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.test\test-resources\negative-tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="285" yWindow="105" windowWidth="16140" windowHeight="9210"/>
+    <workbookView xWindow="285" yWindow="105" windowWidth="16140" windowHeight="9210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Rules" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_st1">#REF!</definedName>
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="32">
   <si>
     <t>operation</t>
   </si>
@@ -56,13 +52,82 @@
   </si>
   <si>
     <t>TBasic Double VariableVisibilityTest()</t>
+  </si>
+  <si>
+    <t>TBasic Double whileVariable()</t>
+  </si>
+  <si>
+    <t>TBasic Double ifVariable()</t>
+  </si>
+  <si>
+    <t>WHILE</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>VAR</t>
+  </si>
+  <si>
+    <t>premium</t>
+  </si>
+  <si>
+    <t>1.3 * 1.4</t>
+  </si>
+  <si>
+    <t>new Double(1.3) * 1.4</t>
+  </si>
+  <si>
+    <t>// Important to have some calculations</t>
+  </si>
+  <si>
+    <t>END WHILE</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>premium * 1.55</t>
+  </si>
+  <si>
+    <t>// Expected to fail because of absent premium variable</t>
+  </si>
+  <si>
+    <t>TBasic Double elseVariable()</t>
+  </si>
+  <si>
+    <t>TBasic Double forEachVariable()</t>
+  </si>
+  <si>
+    <t>nums</t>
+  </si>
+  <si>
+    <t>new Integer[]{5,6,7,8}</t>
+  </si>
+  <si>
+    <t>premium1</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>FOR EACH</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>ELSE</t>
+  </si>
+  <si>
+    <t>new Double(1.3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -80,8 +145,26 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,8 +183,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -124,11 +213,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -136,9 +237,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent1 5 2 2 2 2" xfId="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -534,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -590,4 +707,317 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:J22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="2:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="11"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="F14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="2:10" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="13.5" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="F19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="F14:H14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix failed testes running under Java 11
because of new Double() has been deprecated in Java 11
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/NonExistingVariableInTBasic.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/NonExistingVariableInTBasic.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="30">
   <si>
     <t>operation</t>
   </si>
@@ -75,9 +75,6 @@
     <t>1.3 * 1.4</t>
   </si>
   <si>
-    <t>new Double(1.3) * 1.4</t>
-  </si>
-  <si>
     <t>// Important to have some calculations</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
   </si>
   <si>
     <t>ELSE</t>
-  </si>
-  <si>
-    <t>new Double(1.3)</t>
   </si>
 </sst>
 </file>
@@ -234,12 +228,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -252,6 +240,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1 5 2 2 2 2" xfId="1"/>
@@ -663,11 +657,11 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
@@ -714,7 +708,7 @@
   <dimension ref="B3:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -728,54 +722,54 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="F3" s="5" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="F3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="2:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -794,44 +788,44 @@
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
         <v>16</v>
       </c>
-      <c r="J7" t="s">
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="7"/>
       <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
         <v>19</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>20</v>
-      </c>
-      <c r="J8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -839,16 +833,16 @@
         <v>13</v>
       </c>
       <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
       </c>
       <c r="F9" t="s">
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
@@ -856,59 +850,59 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="D10" s="9"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="F14" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="F14" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="2:10" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -923,65 +917,65 @@
         <v>13</v>
       </c>
       <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" t="s">
         <v>24</v>
       </c>
-      <c r="H17" t="s">
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="F18" t="s">
         <v>27</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>28</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="F19" s="8" t="s">
+      <c r="D19" s="7"/>
+      <c r="F19" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G19" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="9" t="s">
-        <v>31</v>
+      <c r="H19" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>27</v>
+      <c r="D20" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="F20" t="s">
         <v>13</v>
       </c>
       <c r="G20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" t="s">
         <v>19</v>
-      </c>
-      <c r="H20" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
@@ -989,27 +983,27 @@
         <v>13</v>
       </c>
       <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
         <v>19</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
       </c>
       <c r="F21" t="s">
         <v>6</v>
       </c>
       <c r="G21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="11"/>
+        <v>18</v>
+      </c>
+      <c r="D22" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>